<commit_message>
updated Table_Deviance_Explained_2022-03-08 with a field called Label for graphics
</commit_message>
<xml_diff>
--- a/data/Table1_DevianceExp_20220308.xlsx
+++ b/data/Table1_DevianceExp_20220308.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhmockrin\Box\_Workspace\Proj_GitHub22\La_wui\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhmockrin\AppData\Local\Box\Box Edit\Documents\ACqcmZWt_kGsSB+tnw+RHA==\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C3A57A-B350-4B5C-9017-6A8007312CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F01E3A-6713-47E4-B885-06EC9C34739E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Formatted!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Formatted!$A$1:$U$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="178">
   <si>
     <t>Variable name</t>
   </si>
@@ -518,6 +518,57 @@
   </si>
   <si>
     <t>Parcel land cover- percent non vegetated</t>
+  </si>
+  <si>
+    <t>in RF no DINS top 20</t>
+  </si>
+  <si>
+    <t>in RF DINS top 20</t>
+  </si>
+  <si>
+    <t>build_p_otherpaved_200</t>
+  </si>
+  <si>
+    <t>build_p_otherpaved_300</t>
+  </si>
+  <si>
+    <t>build_Mean_distroad</t>
+  </si>
+  <si>
+    <t>build_Mean_elev_30m</t>
+  </si>
+  <si>
+    <t>build_Mean_elev_100m</t>
+  </si>
+  <si>
+    <t>build_Mean_builddens</t>
+  </si>
+  <si>
+    <t>build_p_building_300</t>
+  </si>
+  <si>
+    <t>build_p_tree_300</t>
+  </si>
+  <si>
+    <t>build_p_building_200</t>
+  </si>
+  <si>
+    <t>top Dev</t>
+  </si>
+  <si>
+    <t>build_Mean_slope_100m_DEM</t>
+  </si>
+  <si>
+    <t>build_p_building_100</t>
+  </si>
+  <si>
+    <t>build_p_grass_300</t>
+  </si>
+  <si>
+    <t>build_p_soil_200</t>
+  </si>
+  <si>
+    <t>build_p_tree_100</t>
   </si>
 </sst>
 </file>
@@ -1111,16 +1162,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>589577</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>256202</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>123588</xdr:rowOff>
+      <xdr:rowOff>18813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1143,7 +1194,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20031075" y="1466850"/>
+          <a:off x="23964900" y="1362075"/>
           <a:ext cx="7780952" cy="1895238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1453,10 +1504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U72"/>
+  <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1521,7 @@
     <col min="14" max="18" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>115</v>
       </c>
@@ -1495,8 +1546,17 @@
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" t="s">
+        <v>161</v>
+      </c>
+      <c r="K1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1521,9 +1581,19 @@
       <c r="H2" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="N2"/>
       <c r="S2" s="8"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1548,9 +1618,16 @@
       <c r="H3" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="N3"/>
       <c r="S3" s="8"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1575,8 +1652,9 @@
       <c r="H4" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1601,8 +1679,15 @@
       <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1627,9 +1712,10 @@
       <c r="H6" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="N6"/>
       <c r="S6" s="8"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1654,141 +1740,161 @@
       <c r="H7" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="N7"/>
       <c r="S7" s="8"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F8" s="3">
-        <v>0.21</v>
+        <v>0.01</v>
       </c>
       <c r="G8" s="2">
-        <v>948</v>
+        <v>10126</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="N8"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
       </c>
       <c r="F9" s="3">
-        <v>2.14</v>
+        <v>0.21</v>
       </c>
       <c r="G9" s="2">
-        <v>1069</v>
+        <v>948</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="S9" s="8"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>90</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" s="3">
-        <v>0.54</v>
+        <v>2.14</v>
       </c>
       <c r="G10" s="2">
-        <v>418</v>
+        <v>1069</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>5</v>
       </c>
       <c r="F11" s="3">
-        <v>4.79</v>
+        <v>0.54</v>
       </c>
       <c r="G11" s="2">
-        <v>571</v>
+        <v>418</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>116</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F12" s="3">
-        <v>0.01</v>
+        <v>4.79</v>
       </c>
       <c r="G12" s="2">
-        <v>10126</v>
+        <v>571</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="S12" s="8"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1815,7 +1921,7 @@
       </c>
       <c r="S13" s="8"/>
     </row>
-    <row r="14" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1842,8 +1948,9 @@
       </c>
       <c r="K14"/>
       <c r="U14"/>
-    </row>
-    <row r="15" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W14"/>
+    </row>
+    <row r="15" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1868,10 +1975,13 @@
       <c r="H15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K15"/>
+      <c r="K15">
+        <v>1</v>
+      </c>
       <c r="S15" s="9"/>
-    </row>
-    <row r="16" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W15"/>
+    </row>
+    <row r="16" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1898,8 +2008,9 @@
       </c>
       <c r="K16"/>
       <c r="S16" s="9"/>
-    </row>
-    <row r="17" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W16"/>
+    </row>
+    <row r="17" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1925,9 +2036,11 @@
         <v>46</v>
       </c>
       <c r="K17"/>
+      <c r="N17"/>
       <c r="S17" s="9"/>
-    </row>
-    <row r="18" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W17"/>
+    </row>
+    <row r="18" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1953,9 +2066,11 @@
         <v>46</v>
       </c>
       <c r="K18"/>
+      <c r="N18"/>
       <c r="S18" s="9"/>
-    </row>
-    <row r="19" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W18"/>
+    </row>
+    <row r="19" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1981,9 +2096,11 @@
         <v>46</v>
       </c>
       <c r="K19"/>
+      <c r="N19"/>
       <c r="S19" s="9"/>
-    </row>
-    <row r="20" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W19"/>
+    </row>
+    <row r="20" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2009,9 +2126,11 @@
         <v>46</v>
       </c>
       <c r="K20"/>
+      <c r="N20"/>
       <c r="S20" s="9"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="W20"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2036,9 +2155,10 @@
       <c r="H21" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="N21"/>
       <c r="S21" s="8"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2065,7 +2185,7 @@
       </c>
       <c r="S22" s="8"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2092,7 +2212,7 @@
       </c>
       <c r="S23" s="8"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2119,24 +2239,24 @@
       </c>
       <c r="S24" s="8"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
-        <v>141</v>
+        <v>16</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F25" s="3">
-        <v>0.83</v>
+        <v>7.01</v>
       </c>
       <c r="G25" s="2">
         <v>11134</v>
@@ -2144,26 +2264,32 @@
       <c r="H25" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
       <c r="S25" s="8"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" t="s">
-        <v>150</v>
+        <v>22</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F26" s="3">
-        <v>0.02</v>
+        <v>2.73</v>
       </c>
       <c r="G26" s="2">
         <v>11134</v>
@@ -2171,80 +2297,98 @@
       <c r="H26" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
       <c r="S26" s="8"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="G27" s="6">
-        <v>11087</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="3">
+        <v>3.19</v>
+      </c>
+      <c r="G27" s="2">
+        <v>11134</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
       </c>
       <c r="S27" s="8"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F28" s="5">
-        <v>0.31</v>
-      </c>
-      <c r="G28" s="6">
-        <v>11087</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>46</v>
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="3">
+        <v>3.76</v>
+      </c>
+      <c r="G28" s="2">
+        <v>11134</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
       </c>
       <c r="S28" s="8"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>17</v>
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="3">
-        <v>7.01</v>
+        <v>0.13</v>
       </c>
       <c r="G29" s="2">
         <v>11134</v>
@@ -2254,24 +2398,24 @@
       </c>
       <c r="S29" s="8"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
       </c>
       <c r="F30" s="3">
-        <v>2.73</v>
+        <v>1.75</v>
       </c>
       <c r="G30" s="2">
         <v>11134</v>
@@ -2281,24 +2425,24 @@
       </c>
       <c r="S30" s="8"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
       </c>
       <c r="E31" t="s">
         <v>15</v>
       </c>
       <c r="F31" s="3">
-        <v>3.19</v>
+        <v>1.27</v>
       </c>
       <c r="G31" s="2">
         <v>11134</v>
@@ -2308,24 +2452,24 @@
       </c>
       <c r="S31" s="8"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="E32" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="3">
-        <v>3.76</v>
+        <v>0.1</v>
       </c>
       <c r="G32" s="2">
         <v>11134</v>
@@ -2337,76 +2481,85 @@
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" t="s">
-        <v>32</v>
+        <v>14</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>160</v>
       </c>
       <c r="E33" t="s">
         <v>15</v>
       </c>
       <c r="F33" s="3">
-        <v>0.13</v>
+        <v>7.54</v>
       </c>
       <c r="G33" s="2">
         <v>11134</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
       </c>
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>126</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F34" s="3">
-        <v>1.75</v>
+        <v>3.71</v>
       </c>
       <c r="G34" s="2">
         <v>11134</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
       </c>
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>26</v>
+        <v>68</v>
       </c>
       <c r="D35" t="s">
-        <v>27</v>
+        <v>141</v>
       </c>
       <c r="E35" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F35" s="3">
-        <v>1.27</v>
+        <v>0.83</v>
       </c>
       <c r="G35" s="2">
         <v>11134</v>
@@ -2418,22 +2571,22 @@
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="D36" t="s">
-        <v>35</v>
+        <v>150</v>
       </c>
       <c r="E36" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F36" s="3">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="G36" s="2">
         <v>11134</v>
@@ -2445,238 +2598,271 @@
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>117</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>14</v>
+        <v>96</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E37" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="3">
-        <v>7.54</v>
-      </c>
-      <c r="G37" s="2">
-        <v>11134</v>
-      </c>
-      <c r="H37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="G37" s="6">
+        <v>11087</v>
+      </c>
+      <c r="H37" s="7" t="s">
         <v>46</v>
       </c>
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D38" t="s">
-        <v>126</v>
-      </c>
-      <c r="E38" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" s="3">
-        <v>3.71</v>
-      </c>
-      <c r="G38" s="2">
-        <v>11134</v>
-      </c>
-      <c r="H38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0.31</v>
+      </c>
+      <c r="G38" s="6">
+        <v>11087</v>
+      </c>
+      <c r="H38" s="7" t="s">
         <v>46</v>
       </c>
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="E39" t="s">
         <v>5</v>
       </c>
       <c r="F39" s="3">
-        <v>4.82</v>
+        <v>2.2599999999999998</v>
       </c>
       <c r="G39" s="2">
-        <v>11134</v>
+        <v>11046</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>46</v>
+        <v>83</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>1</v>
       </c>
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="D40" t="s">
-        <v>122</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
         <v>5</v>
       </c>
       <c r="F40" s="3">
-        <v>5.18</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="G40" s="2">
-        <v>11134</v>
+        <v>11122</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="D41" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="E41" t="s">
         <v>5</v>
       </c>
       <c r="F41" s="3">
-        <v>2.0499999999999998</v>
+        <v>1.29</v>
       </c>
       <c r="G41" s="2">
-        <v>11134</v>
+        <v>11046</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>46</v>
+        <v>83</v>
+      </c>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
       </c>
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E42" t="s">
         <v>5</v>
       </c>
       <c r="F42" s="3">
-        <v>2.81</v>
+        <v>4.82</v>
       </c>
       <c r="G42" s="2">
         <v>11134</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
       </c>
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E43" t="s">
         <v>5</v>
       </c>
       <c r="F43" s="3">
-        <v>3.43</v>
+        <v>5.18</v>
       </c>
       <c r="G43" s="2">
         <v>11134</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
       </c>
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D44" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="E44" t="s">
         <v>5</v>
       </c>
       <c r="F44" s="3">
-        <v>3.04</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="G44" s="2">
         <v>11134</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
       </c>
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="D45" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E45" t="s">
         <v>5</v>
       </c>
       <c r="F45" s="3">
-        <v>4.8</v>
+        <v>2.81</v>
       </c>
       <c r="G45" s="2">
         <v>11134</v>
@@ -2684,26 +2870,30 @@
       <c r="H45" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="O45"/>
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D46" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E46" t="s">
         <v>5</v>
       </c>
       <c r="F46" s="3">
-        <v>5.75</v>
+        <v>3.43</v>
       </c>
       <c r="G46" s="2">
         <v>11134</v>
@@ -2711,26 +2901,33 @@
       <c r="H46" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="O46"/>
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E47" t="s">
         <v>5</v>
       </c>
       <c r="F47" s="3">
-        <v>2.21</v>
+        <v>3.04</v>
       </c>
       <c r="G47" s="2">
         <v>11134</v>
@@ -2738,26 +2935,30 @@
       <c r="H47" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="O47"/>
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D48" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E48" t="s">
         <v>5</v>
       </c>
       <c r="F48" s="3">
-        <v>3.1</v>
+        <v>4.8</v>
       </c>
       <c r="G48" s="2">
         <v>11134</v>
@@ -2765,26 +2966,36 @@
       <c r="H48" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="O48"/>
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E49" t="s">
         <v>5</v>
       </c>
       <c r="F49" s="3">
-        <v>4.01</v>
+        <v>5.75</v>
       </c>
       <c r="G49" s="2">
         <v>11134</v>
@@ -2792,26 +3003,36 @@
       <c r="H49" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="O49"/>
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D50" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="E50" t="s">
         <v>5</v>
       </c>
       <c r="F50" s="3">
-        <v>0.12</v>
+        <v>2.21</v>
       </c>
       <c r="G50" s="2">
         <v>11134</v>
@@ -2819,26 +3040,27 @@
       <c r="H50" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="O50"/>
       <c r="S50" s="8"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D51" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E51" t="s">
         <v>5</v>
       </c>
       <c r="F51" s="3">
-        <v>0.52</v>
+        <v>3.1</v>
       </c>
       <c r="G51" s="2">
         <v>11134</v>
@@ -2846,26 +3068,30 @@
       <c r="H51" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="O51"/>
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D52" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E52" t="s">
         <v>5</v>
       </c>
       <c r="F52" s="3">
-        <v>1.07</v>
+        <v>4.01</v>
       </c>
       <c r="G52" s="2">
         <v>11134</v>
@@ -2873,26 +3099,30 @@
       <c r="H52" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="O52"/>
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E53" t="s">
         <v>5</v>
       </c>
       <c r="F53" s="3">
-        <v>2.2000000000000002</v>
+        <v>0.12</v>
       </c>
       <c r="G53" s="2">
         <v>11134</v>
@@ -2904,22 +3134,22 @@
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D54" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="E54" t="s">
         <v>5</v>
       </c>
       <c r="F54" s="3">
-        <v>2.68</v>
+        <v>0.52</v>
       </c>
       <c r="G54" s="2">
         <v>11134</v>
@@ -2931,22 +3161,22 @@
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D55" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="E55" t="s">
         <v>5</v>
       </c>
       <c r="F55" s="3">
-        <v>2.2799999999999998</v>
+        <v>1.07</v>
       </c>
       <c r="G55" s="2">
         <v>11134</v>
@@ -2958,22 +3188,22 @@
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="E56" t="s">
         <v>5</v>
       </c>
       <c r="F56" s="3">
-        <v>2.54</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G56" s="2">
         <v>11134</v>
@@ -2985,49 +3215,52 @@
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D57" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E57" t="s">
         <v>5</v>
       </c>
       <c r="F57" s="3">
-        <v>2.2400000000000002</v>
+        <v>2.68</v>
       </c>
       <c r="G57" s="2">
         <v>11134</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
       </c>
       <c r="S57" s="8"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D58" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E58" t="s">
         <v>5</v>
       </c>
       <c r="F58" s="3">
-        <v>2.44</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="G58" s="2">
         <v>11134</v>
@@ -3039,103 +3272,115 @@
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D59" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="E59" t="s">
         <v>5</v>
       </c>
       <c r="F59" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>2.54</v>
       </c>
       <c r="G59" s="2">
         <v>11134</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
       </c>
       <c r="S59" s="8"/>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="D60" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="E60" t="s">
         <v>5</v>
       </c>
       <c r="F60" s="3">
-        <v>0.03</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="G60" s="2">
         <v>11134</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
       </c>
       <c r="S60" s="8"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="D61" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="E61" t="s">
         <v>5</v>
       </c>
       <c r="F61" s="3">
-        <v>0.04</v>
+        <v>2.44</v>
       </c>
       <c r="G61" s="2">
         <v>11134</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
       </c>
       <c r="S61" s="8"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D62" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="E62" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F62" s="3">
-        <v>0.32</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G62" s="2">
         <v>11134</v>
@@ -3147,82 +3392,82 @@
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D63" t="s">
-        <v>39</v>
+        <v>149</v>
       </c>
       <c r="E63" t="s">
         <v>5</v>
       </c>
       <c r="F63" s="3">
-        <v>2.2599999999999998</v>
+        <v>0.03</v>
       </c>
       <c r="G63" s="2">
-        <v>11046</v>
+        <v>11134</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="S63" s="8"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="D64" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E64" t="s">
         <v>5</v>
       </c>
       <c r="F64" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="G64" s="2">
-        <v>11122</v>
+        <v>11134</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="S64" s="8"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="E65" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F65" s="3">
-        <v>1.29</v>
+        <v>0.32</v>
       </c>
       <c r="G65" s="2">
-        <v>11046</v>
+        <v>11134</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="S65" s="8"/>
     </row>
@@ -3305,6 +3550,12 @@
       <c r="H68" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
       <c r="S68" s="8"/>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.25">
@@ -3332,6 +3583,9 @@
       <c r="H69" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
       <c r="S69" s="8"/>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.25">
@@ -3359,6 +3613,12 @@
       <c r="H70" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
       <c r="S70" s="8"/>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.25">
@@ -3386,17 +3646,22 @@
       <c r="H71" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
       <c r="S71" s="8"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="S72" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B15:H36">
-    <sortCondition ref="B15:B36"/>
-    <sortCondition ref="E15:E36"/>
-    <sortCondition ref="C15:C36"/>
+  <autoFilter ref="A1:U71" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U71">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N9:N21">
+    <sortCondition ref="N9:N21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -3406,16 +3671,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A03775-521C-4F2A-B1FE-2F03AF2919BD}">
-  <dimension ref="F27"/>
+  <dimension ref="E13:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:P12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="27" spans="6:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="5:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E27" t="s">
+        <v>175</v>
+      </c>
       <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>177</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>